<commit_message>
updated gantt chart for 6/21/2020
</commit_message>
<xml_diff>
--- a/ai_semiconductors/doc/Ganttchart_data.xlsx
+++ b/ai_semiconductors/doc/Ganttchart_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIRECT\Capstone\ai_semiconductors\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIRECT\Capstone\ai_semiconductors\ai_semiconductors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D050361-7B7B-41FF-A23E-257B0F7A6E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E258B7-5B11-49CE-B926-ACD5C6EB9FB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4290" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
+    <workbookView xWindow="-28920" yWindow="-4290" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39CDD02A-CF22-45E9-9E33-1B53688FC745}"/>
   </bookViews>
   <sheets>
     <sheet name="200413" sheetId="1" r:id="rId1"/>
     <sheet name="200422" sheetId="2" r:id="rId2"/>
     <sheet name="200501" sheetId="3" r:id="rId3"/>
     <sheet name="200515" sheetId="4" r:id="rId4"/>
+    <sheet name="200621" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -126,6 +127,18 @@
   </si>
   <si>
     <t>Uncertainty prediction: all models</t>
+  </si>
+  <si>
+    <t>Continue to work on project for publication</t>
+  </si>
+  <si>
+    <t>Find experimental data values for outputs</t>
+  </si>
+  <si>
+    <t>Build prediction tool</t>
+  </si>
+  <si>
+    <t>Descriptor expansion/selection through SISSO and LASSO</t>
   </si>
 </sst>
 </file>
@@ -968,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502BF6A5-AB71-4B0F-8CC4-AE47241D155F}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1221,4 +1234,305 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F5463B-D28A-499C-BEFF-6372E0978C4D}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="56.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.2265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43934</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43943</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43973</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43957</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43957</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43992</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43976</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43992</v>
+      </c>
+      <c r="D18" s="2">
+        <v>43999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43997</v>
+      </c>
+      <c r="D19" s="2">
+        <v>44006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44006</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44075</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>